<commit_message>
Update to rectify the sample ID columns
</commit_message>
<xml_diff>
--- a/public/docs/Edarp2.xlsx
+++ b/public/docs/Edarp2.xlsx
@@ -1,21 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bakasa\code\lab\public\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2668DA7F-48EC-4446-B7F5-FCC050AF0904}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
+  <calcPr calcId="191029" forceFullCalc="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1970" uniqueCount="137">
   <si>
     <t>Type</t>
   </si>
@@ -260,9 +272,6 @@
     <t>05/10/2019 00:00:01 AM</t>
   </si>
   <si>
-    <t>1022953R</t>
-  </si>
-  <si>
     <t>05/10/2019 07:33:07 AM</t>
   </si>
   <si>
@@ -287,9 +296,6 @@
     <t>72 cp/ml</t>
   </si>
   <si>
-    <t>1022930R</t>
-  </si>
-  <si>
     <t>120 cp/ml</t>
   </si>
   <si>
@@ -302,81 +308,48 @@
     <t>05/09/2019 21:49:53 PM</t>
   </si>
   <si>
-    <t>1022935R</t>
-  </si>
-  <si>
-    <t>1022944R</t>
-  </si>
-  <si>
     <t>6723 cp/ml</t>
   </si>
   <si>
     <t>1740 cp/ml</t>
   </si>
   <si>
-    <t>1022941R</t>
-  </si>
-  <si>
     <t>56 cp/ml</t>
   </si>
   <si>
     <t>51910 cp/ml</t>
   </si>
   <si>
-    <t>1022939R</t>
-  </si>
-  <si>
     <t>2907 cp/ml</t>
   </si>
   <si>
     <t>558 cp/ml</t>
   </si>
   <si>
-    <t>1022942R</t>
-  </si>
-  <si>
     <t>1397 cp/ml</t>
   </si>
   <si>
-    <t>1022933R</t>
-  </si>
-  <si>
     <t>577 cp/ml</t>
   </si>
   <si>
     <t>9202 cp/ml</t>
   </si>
   <si>
-    <t>1022938R</t>
-  </si>
-  <si>
     <t>43 cp/ml</t>
   </si>
   <si>
-    <t>1022940R</t>
-  </si>
-  <si>
     <t>2603 cp/ml</t>
   </si>
   <si>
-    <t>1022927R</t>
-  </si>
-  <si>
     <t>268 cp/ml</t>
   </si>
   <si>
     <t>386872 cp/ml</t>
   </si>
   <si>
-    <t>1022928R</t>
-  </si>
-  <si>
     <t>869 cp/ml</t>
   </si>
   <si>
-    <t>1022932R</t>
-  </si>
-  <si>
     <t>351 cp/ml</t>
   </si>
   <si>
@@ -395,42 +368,27 @@
     <t>295708 cp/ml</t>
   </si>
   <si>
-    <t>1022949R</t>
-  </si>
-  <si>
     <t>2526 cp/ml</t>
   </si>
   <si>
     <t>358492 cp/ml</t>
   </si>
   <si>
-    <t>1022934R</t>
-  </si>
-  <si>
     <t>154 cp/ml</t>
   </si>
   <si>
-    <t>1022946R</t>
-  </si>
-  <si>
     <t>210 cp/ml</t>
   </si>
   <si>
     <t>108 cp/ml</t>
   </si>
   <si>
-    <t>1022929R</t>
-  </si>
-  <si>
     <t>19614 cp/ml</t>
   </si>
   <si>
     <t>321623 cp/ml</t>
   </si>
   <si>
-    <t>1022937R</t>
-  </si>
-  <si>
     <t>612 cp/ml</t>
   </si>
   <si>
@@ -446,9 +404,6 @@
     <t>220241 cp/ml</t>
   </si>
   <si>
-    <t>1022943R</t>
-  </si>
-  <si>
     <t>441 cp/ml</t>
   </si>
   <si>
@@ -458,13 +413,7 @@
     <t>513 cp/ml</t>
   </si>
   <si>
-    <t>1022945R</t>
-  </si>
-  <si>
     <t>488 cp/ml</t>
-  </si>
-  <si>
-    <t>1022948R</t>
   </si>
   <si>
     <t>7433 cp/ml</t>
@@ -494,14 +443,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -512,28 +456,37 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -823,19 +776,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N217"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="D210" sqref="D210"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -876,7 +831,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -911,7 +866,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -946,7 +901,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -981,7 +936,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1016,7 +971,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1051,7 +1006,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1083,7 +1038,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1118,7 +1073,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1153,7 +1108,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1188,7 +1143,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1223,7 +1178,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1258,7 +1213,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1290,7 +1245,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1325,7 +1280,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1360,7 +1315,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1395,7 +1350,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1430,7 +1385,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1462,7 +1417,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -1494,7 +1449,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -1529,7 +1484,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -1564,7 +1519,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1599,7 +1554,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1634,7 +1589,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1669,7 +1624,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1701,7 +1656,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -1736,7 +1691,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -1771,7 +1726,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -1806,7 +1761,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -1841,7 +1796,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1873,7 +1828,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -1905,7 +1860,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -1940,7 +1895,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>13</v>
       </c>
@@ -1975,7 +1930,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>13</v>
       </c>
@@ -2010,7 +1965,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -2045,7 +2000,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>13</v>
       </c>
@@ -2080,7 +2035,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>13</v>
       </c>
@@ -2115,7 +2070,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>13</v>
       </c>
@@ -2150,7 +2105,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -2185,7 +2140,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>13</v>
       </c>
@@ -2220,7 +2175,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -2255,7 +2210,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>13</v>
       </c>
@@ -2290,7 +2245,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>13</v>
       </c>
@@ -2325,7 +2280,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>13</v>
       </c>
@@ -2360,7 +2315,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>13</v>
       </c>
@@ -2395,7 +2350,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>13</v>
       </c>
@@ -2430,7 +2385,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>13</v>
       </c>
@@ -2465,7 +2420,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>13</v>
       </c>
@@ -2500,7 +2455,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:14">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>13</v>
       </c>
@@ -2535,7 +2490,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:14">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>13</v>
       </c>
@@ -2570,7 +2525,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:14">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>13</v>
       </c>
@@ -2605,7 +2560,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:14">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>13</v>
       </c>
@@ -2640,7 +2595,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:14">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>30</v>
       </c>
@@ -2672,7 +2627,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:14">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>13</v>
       </c>
@@ -2707,7 +2662,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:14">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>13</v>
       </c>
@@ -2742,7 +2697,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="1:14">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>13</v>
       </c>
@@ -2777,7 +2732,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="57" spans="1:14">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>13</v>
       </c>
@@ -2812,7 +2767,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="58" spans="1:14">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>13</v>
       </c>
@@ -2847,7 +2802,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:14">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>13</v>
       </c>
@@ -2885,7 +2840,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="60" spans="1:14">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>13</v>
       </c>
@@ -2920,7 +2875,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="1:14">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>13</v>
       </c>
@@ -2955,7 +2910,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="62" spans="1:14">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>13</v>
       </c>
@@ -2990,7 +2945,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:14">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>13</v>
       </c>
@@ -3025,7 +2980,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="64" spans="1:14">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>13</v>
       </c>
@@ -3060,7 +3015,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="65" spans="1:14">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>13</v>
       </c>
@@ -3095,7 +3050,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="66" spans="1:14">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>13</v>
       </c>
@@ -3130,7 +3085,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="67" spans="1:14">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>39</v>
       </c>
@@ -3162,7 +3117,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="68" spans="1:14">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>13</v>
       </c>
@@ -3197,7 +3152,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="1:14">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>13</v>
       </c>
@@ -3232,7 +3187,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:14">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>13</v>
       </c>
@@ -3267,7 +3222,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="71" spans="1:14">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>13</v>
       </c>
@@ -3302,7 +3257,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="72" spans="1:14">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>13</v>
       </c>
@@ -3337,7 +3292,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="73" spans="1:14">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>13</v>
       </c>
@@ -3372,7 +3327,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="74" spans="1:14">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>13</v>
       </c>
@@ -3407,7 +3362,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:14">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>13</v>
       </c>
@@ -3442,7 +3397,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:14">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>13</v>
       </c>
@@ -3477,7 +3432,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:14">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>13</v>
       </c>
@@ -3512,7 +3467,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:14">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>13</v>
       </c>
@@ -3547,7 +3502,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="79" spans="1:14">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>13</v>
       </c>
@@ -3582,15 +3537,15 @@
         <v>74</v>
       </c>
     </row>
-    <row r="80" spans="1:14">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>13</v>
       </c>
-      <c r="B80" t="s">
-        <v>81</v>
-      </c>
-      <c r="C80" t="s">
-        <v>81</v>
+      <c r="B80">
+        <v>1022953</v>
+      </c>
+      <c r="C80">
+        <v>1022953</v>
       </c>
       <c r="D80" t="s">
         <v>14</v>
@@ -3602,11 +3557,11 @@
         <v>29</v>
       </c>
       <c r="H80" t="s">
+        <v>81</v>
+      </c>
+      <c r="J80" t="s">
         <v>82</v>
       </c>
-      <c r="J80" t="s">
-        <v>83</v>
-      </c>
       <c r="K80" t="s">
         <v>19</v>
       </c>
@@ -3617,7 +3572,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="81" spans="1:14">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>13</v>
       </c>
@@ -3634,14 +3589,14 @@
         <v>15</v>
       </c>
       <c r="F81" t="s">
+        <v>83</v>
+      </c>
+      <c r="H81" t="s">
         <v>84</v>
       </c>
-      <c r="H81" t="s">
+      <c r="J81" t="s">
         <v>85</v>
       </c>
-      <c r="J81" t="s">
-        <v>86</v>
-      </c>
       <c r="K81" t="s">
         <v>19</v>
       </c>
@@ -3652,7 +3607,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="82" spans="1:14">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>13</v>
       </c>
@@ -3687,7 +3642,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="83" spans="1:14">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>13</v>
       </c>
@@ -3704,14 +3659,14 @@
         <v>15</v>
       </c>
       <c r="F83" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H83" t="s">
+        <v>84</v>
+      </c>
+      <c r="J83" t="s">
         <v>85</v>
       </c>
-      <c r="J83" t="s">
-        <v>86</v>
-      </c>
       <c r="K83" t="s">
         <v>19</v>
       </c>
@@ -3722,7 +3677,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="84" spans="1:14">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>33</v>
       </c>
@@ -3736,14 +3691,14 @@
         <v>15</v>
       </c>
       <c r="F84" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H84" t="s">
+        <v>84</v>
+      </c>
+      <c r="J84" t="s">
         <v>85</v>
       </c>
-      <c r="J84" t="s">
-        <v>86</v>
-      </c>
       <c r="K84" t="s">
         <v>19</v>
       </c>
@@ -3754,7 +3709,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="85" spans="1:14">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>13</v>
       </c>
@@ -3789,7 +3744,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="86" spans="1:14">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>13</v>
       </c>
@@ -3806,7 +3761,7 @@
         <v>15</v>
       </c>
       <c r="F86" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H86" t="s">
         <v>76</v>
@@ -3824,7 +3779,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="87" spans="1:14">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>13</v>
       </c>
@@ -3844,11 +3799,11 @@
         <v>29</v>
       </c>
       <c r="H87" t="s">
+        <v>84</v>
+      </c>
+      <c r="J87" t="s">
         <v>85</v>
       </c>
-      <c r="J87" t="s">
-        <v>86</v>
-      </c>
       <c r="K87" t="s">
         <v>19</v>
       </c>
@@ -3859,15 +3814,15 @@
         <v>74</v>
       </c>
     </row>
-    <row r="88" spans="1:14">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>13</v>
       </c>
-      <c r="B88" t="s">
-        <v>90</v>
-      </c>
-      <c r="C88" t="s">
-        <v>90</v>
+      <c r="B88">
+        <v>1022930</v>
+      </c>
+      <c r="C88">
+        <v>1022930</v>
       </c>
       <c r="D88" t="s">
         <v>14</v>
@@ -3876,14 +3831,14 @@
         <v>15</v>
       </c>
       <c r="F88" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H88" t="s">
+        <v>81</v>
+      </c>
+      <c r="J88" t="s">
         <v>82</v>
       </c>
-      <c r="J88" t="s">
-        <v>83</v>
-      </c>
       <c r="K88" t="s">
         <v>19</v>
       </c>
@@ -3894,7 +3849,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="89" spans="1:14">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>13</v>
       </c>
@@ -3914,11 +3869,11 @@
         <v>29</v>
       </c>
       <c r="H89" t="s">
+        <v>84</v>
+      </c>
+      <c r="J89" t="s">
         <v>85</v>
       </c>
-      <c r="J89" t="s">
-        <v>86</v>
-      </c>
       <c r="K89" t="s">
         <v>19</v>
       </c>
@@ -3929,7 +3884,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="90" spans="1:14">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>13</v>
       </c>
@@ -3946,7 +3901,7 @@
         <v>15</v>
       </c>
       <c r="F90" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H90" t="s">
         <v>72</v>
@@ -3964,7 +3919,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="91" spans="1:14">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>13</v>
       </c>
@@ -3984,10 +3939,10 @@
         <v>69</v>
       </c>
       <c r="H91" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J91" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K91" t="s">
         <v>19</v>
@@ -3999,15 +3954,15 @@
         <v>74</v>
       </c>
     </row>
-    <row r="92" spans="1:14">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>13</v>
       </c>
-      <c r="B92" t="s">
-        <v>95</v>
-      </c>
-      <c r="C92" t="s">
-        <v>95</v>
+      <c r="B92">
+        <v>1022935</v>
+      </c>
+      <c r="C92">
+        <v>1022935</v>
       </c>
       <c r="D92" t="s">
         <v>14</v>
@@ -4019,11 +3974,11 @@
         <v>25</v>
       </c>
       <c r="H92" t="s">
+        <v>81</v>
+      </c>
+      <c r="J92" t="s">
         <v>82</v>
       </c>
-      <c r="J92" t="s">
-        <v>83</v>
-      </c>
       <c r="K92" t="s">
         <v>19</v>
       </c>
@@ -4034,7 +3989,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="93" spans="1:14">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>13</v>
       </c>
@@ -4054,11 +4009,11 @@
         <v>29</v>
       </c>
       <c r="H93" t="s">
+        <v>84</v>
+      </c>
+      <c r="J93" t="s">
         <v>85</v>
       </c>
-      <c r="J93" t="s">
-        <v>86</v>
-      </c>
       <c r="K93" t="s">
         <v>19</v>
       </c>
@@ -4069,7 +4024,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="94" spans="1:14">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>13</v>
       </c>
@@ -4104,7 +4059,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="95" spans="1:14">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>13</v>
       </c>
@@ -4124,46 +4079,46 @@
         <v>25</v>
       </c>
       <c r="H95" t="s">
+        <v>91</v>
+      </c>
+      <c r="J95" t="s">
+        <v>92</v>
+      </c>
+      <c r="K95" t="s">
+        <v>19</v>
+      </c>
+      <c r="L95" t="s">
+        <v>20</v>
+      </c>
+      <c r="M95" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>13</v>
+      </c>
+      <c r="B96">
+        <v>1022944</v>
+      </c>
+      <c r="C96">
+        <v>1022944</v>
+      </c>
+      <c r="D96" t="s">
+        <v>14</v>
+      </c>
+      <c r="E96" t="s">
+        <v>15</v>
+      </c>
+      <c r="F96" t="s">
         <v>93</v>
       </c>
-      <c r="J95" t="s">
-        <v>94</v>
-      </c>
-      <c r="K95" t="s">
-        <v>19</v>
-      </c>
-      <c r="L95" t="s">
-        <v>20</v>
-      </c>
-      <c r="M95" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="96" spans="1:14">
-      <c r="A96" t="s">
-        <v>13</v>
-      </c>
-      <c r="B96" t="s">
-        <v>96</v>
-      </c>
-      <c r="C96" t="s">
-        <v>96</v>
-      </c>
-      <c r="D96" t="s">
-        <v>14</v>
-      </c>
-      <c r="E96" t="s">
-        <v>15</v>
-      </c>
-      <c r="F96" t="s">
-        <v>97</v>
-      </c>
       <c r="H96" t="s">
+        <v>81</v>
+      </c>
+      <c r="J96" t="s">
         <v>82</v>
       </c>
-      <c r="J96" t="s">
-        <v>83</v>
-      </c>
       <c r="K96" t="s">
         <v>19</v>
       </c>
@@ -4174,7 +4129,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="97" spans="1:14">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>13</v>
       </c>
@@ -4209,7 +4164,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="98" spans="1:14">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>13</v>
       </c>
@@ -4244,7 +4199,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="99" spans="1:14">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>13</v>
       </c>
@@ -4264,10 +4219,10 @@
         <v>29</v>
       </c>
       <c r="H99" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J99" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K99" t="s">
         <v>19</v>
@@ -4279,7 +4234,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="100" spans="1:14">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>13</v>
       </c>
@@ -4299,10 +4254,10 @@
         <v>25</v>
       </c>
       <c r="H100" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J100" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K100" t="s">
         <v>19</v>
@@ -4314,7 +4269,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="101" spans="1:14">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>13</v>
       </c>
@@ -4331,7 +4286,7 @@
         <v>15</v>
       </c>
       <c r="F101" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H101" t="s">
         <v>72</v>
@@ -4349,7 +4304,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="102" spans="1:14">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>13</v>
       </c>
@@ -4369,11 +4324,11 @@
         <v>29</v>
       </c>
       <c r="H102" t="s">
+        <v>84</v>
+      </c>
+      <c r="J102" t="s">
         <v>85</v>
       </c>
-      <c r="J102" t="s">
-        <v>86</v>
-      </c>
       <c r="K102" t="s">
         <v>19</v>
       </c>
@@ -4384,15 +4339,15 @@
         <v>74</v>
       </c>
     </row>
-    <row r="103" spans="1:14">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>13</v>
       </c>
-      <c r="B103" t="s">
-        <v>99</v>
-      </c>
-      <c r="C103" t="s">
-        <v>99</v>
+      <c r="B103">
+        <v>1022941</v>
+      </c>
+      <c r="C103">
+        <v>1022941</v>
       </c>
       <c r="D103" t="s">
         <v>14</v>
@@ -4401,14 +4356,14 @@
         <v>15</v>
       </c>
       <c r="F103" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H103" t="s">
+        <v>81</v>
+      </c>
+      <c r="J103" t="s">
         <v>82</v>
       </c>
-      <c r="J103" t="s">
-        <v>83</v>
-      </c>
       <c r="K103" t="s">
         <v>19</v>
       </c>
@@ -4419,7 +4374,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="104" spans="1:14">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>13</v>
       </c>
@@ -4454,7 +4409,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="105" spans="1:14">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>13</v>
       </c>
@@ -4474,11 +4429,11 @@
         <v>25</v>
       </c>
       <c r="H105" t="s">
+        <v>84</v>
+      </c>
+      <c r="J105" t="s">
         <v>85</v>
       </c>
-      <c r="J105" t="s">
-        <v>86</v>
-      </c>
       <c r="K105" t="s">
         <v>19</v>
       </c>
@@ -4489,7 +4444,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="106" spans="1:14">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>13</v>
       </c>
@@ -4509,10 +4464,10 @@
         <v>25</v>
       </c>
       <c r="H106" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J106" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K106" t="s">
         <v>19</v>
@@ -4524,7 +4479,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="107" spans="1:14">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>13</v>
       </c>
@@ -4541,7 +4496,7 @@
         <v>15</v>
       </c>
       <c r="F107" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H107" t="s">
         <v>79</v>
@@ -4559,15 +4514,15 @@
         <v>74</v>
       </c>
     </row>
-    <row r="108" spans="1:14">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>13</v>
       </c>
-      <c r="B108" t="s">
-        <v>102</v>
-      </c>
-      <c r="C108" t="s">
-        <v>102</v>
+      <c r="B108">
+        <v>1022939</v>
+      </c>
+      <c r="C108">
+        <v>1022939</v>
       </c>
       <c r="D108" t="s">
         <v>14</v>
@@ -4576,14 +4531,14 @@
         <v>15</v>
       </c>
       <c r="F108" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H108" t="s">
+        <v>81</v>
+      </c>
+      <c r="J108" t="s">
         <v>82</v>
       </c>
-      <c r="J108" t="s">
-        <v>83</v>
-      </c>
       <c r="K108" t="s">
         <v>19</v>
       </c>
@@ -4594,7 +4549,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="109" spans="1:14">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>30</v>
       </c>
@@ -4611,10 +4566,10 @@
         <v>25</v>
       </c>
       <c r="H109" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J109" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K109" t="s">
         <v>19</v>
@@ -4626,7 +4581,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="110" spans="1:14">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>13</v>
       </c>
@@ -4643,7 +4598,7 @@
         <v>15</v>
       </c>
       <c r="F110" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="H110" t="s">
         <v>79</v>
@@ -4661,15 +4616,15 @@
         <v>74</v>
       </c>
     </row>
-    <row r="111" spans="1:14">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>13</v>
       </c>
-      <c r="B111" t="s">
-        <v>105</v>
-      </c>
-      <c r="C111" t="s">
-        <v>105</v>
+      <c r="B111">
+        <v>1022942</v>
+      </c>
+      <c r="C111">
+        <v>1022942</v>
       </c>
       <c r="D111" t="s">
         <v>14</v>
@@ -4678,14 +4633,14 @@
         <v>15</v>
       </c>
       <c r="F111" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="H111" t="s">
+        <v>81</v>
+      </c>
+      <c r="J111" t="s">
         <v>82</v>
       </c>
-      <c r="J111" t="s">
-        <v>83</v>
-      </c>
       <c r="K111" t="s">
         <v>19</v>
       </c>
@@ -4696,15 +4651,15 @@
         <v>74</v>
       </c>
     </row>
-    <row r="112" spans="1:14">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>13</v>
       </c>
-      <c r="B112" t="s">
-        <v>107</v>
-      </c>
-      <c r="C112" t="s">
-        <v>107</v>
+      <c r="B112">
+        <v>1022933</v>
+      </c>
+      <c r="C112">
+        <v>1022933</v>
       </c>
       <c r="D112" t="s">
         <v>14</v>
@@ -4716,11 +4671,11 @@
         <v>29</v>
       </c>
       <c r="H112" t="s">
+        <v>81</v>
+      </c>
+      <c r="J112" t="s">
         <v>82</v>
       </c>
-      <c r="J112" t="s">
-        <v>83</v>
-      </c>
       <c r="K112" t="s">
         <v>19</v>
       </c>
@@ -4731,7 +4686,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="113" spans="1:14">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>13</v>
       </c>
@@ -4766,7 +4721,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="114" spans="1:14">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>33</v>
       </c>
@@ -4780,7 +4735,7 @@
         <v>15</v>
       </c>
       <c r="F114" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="H114" t="s">
         <v>79</v>
@@ -4798,7 +4753,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="115" spans="1:14">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>13</v>
       </c>
@@ -4833,7 +4788,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="116" spans="1:14">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>13</v>
       </c>
@@ -4868,7 +4823,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="117" spans="1:14">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>13</v>
       </c>
@@ -4888,11 +4843,11 @@
         <v>29</v>
       </c>
       <c r="H117" t="s">
+        <v>84</v>
+      </c>
+      <c r="J117" t="s">
         <v>85</v>
       </c>
-      <c r="J117" t="s">
-        <v>86</v>
-      </c>
       <c r="K117" t="s">
         <v>19</v>
       </c>
@@ -4903,7 +4858,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="118" spans="1:14">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>13</v>
       </c>
@@ -4938,7 +4893,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="119" spans="1:14">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>13</v>
       </c>
@@ -4973,7 +4928,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="120" spans="1:14">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>13</v>
       </c>
@@ -4990,7 +4945,7 @@
         <v>15</v>
       </c>
       <c r="F120" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="H120" t="s">
         <v>76</v>
@@ -5008,7 +4963,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="121" spans="1:14">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>13</v>
       </c>
@@ -5043,15 +4998,15 @@
         <v>74</v>
       </c>
     </row>
-    <row r="122" spans="1:14">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>13</v>
       </c>
-      <c r="B122" t="s">
-        <v>110</v>
-      </c>
-      <c r="C122" t="s">
-        <v>110</v>
+      <c r="B122">
+        <v>1022938</v>
+      </c>
+      <c r="C122">
+        <v>1022938</v>
       </c>
       <c r="D122" t="s">
         <v>14</v>
@@ -5063,11 +5018,11 @@
         <v>29</v>
       </c>
       <c r="H122" t="s">
+        <v>81</v>
+      </c>
+      <c r="J122" t="s">
         <v>82</v>
       </c>
-      <c r="J122" t="s">
-        <v>83</v>
-      </c>
       <c r="K122" t="s">
         <v>19</v>
       </c>
@@ -5078,7 +5033,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="123" spans="1:14">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>13</v>
       </c>
@@ -5098,11 +5053,11 @@
         <v>25</v>
       </c>
       <c r="H123" t="s">
+        <v>84</v>
+      </c>
+      <c r="J123" t="s">
         <v>85</v>
       </c>
-      <c r="J123" t="s">
-        <v>86</v>
-      </c>
       <c r="K123" t="s">
         <v>19</v>
       </c>
@@ -5113,7 +5068,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="124" spans="1:14">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>13</v>
       </c>
@@ -5148,7 +5103,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="125" spans="1:14">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>13</v>
       </c>
@@ -5183,7 +5138,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="126" spans="1:14">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>13</v>
       </c>
@@ -5203,10 +5158,10 @@
         <v>44</v>
       </c>
       <c r="H126" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J126" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K126" t="s">
         <v>19</v>
@@ -5218,7 +5173,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="127" spans="1:14">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>13</v>
       </c>
@@ -5238,10 +5193,10 @@
         <v>29</v>
       </c>
       <c r="H127" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J127" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K127" t="s">
         <v>19</v>
@@ -5253,7 +5208,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="128" spans="1:14">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>13</v>
       </c>
@@ -5270,7 +5225,7 @@
         <v>15</v>
       </c>
       <c r="F128" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="H128" t="s">
         <v>79</v>
@@ -5288,7 +5243,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="129" spans="1:14">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>13</v>
       </c>
@@ -5323,15 +5278,15 @@
         <v>74</v>
       </c>
     </row>
-    <row r="130" spans="1:14">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>13</v>
       </c>
-      <c r="B130" t="s">
-        <v>112</v>
-      </c>
-      <c r="C130" t="s">
-        <v>112</v>
+      <c r="B130">
+        <v>1022940</v>
+      </c>
+      <c r="C130">
+        <v>1022940</v>
       </c>
       <c r="D130" t="s">
         <v>14</v>
@@ -5340,14 +5295,14 @@
         <v>15</v>
       </c>
       <c r="F130" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="H130" t="s">
+        <v>81</v>
+      </c>
+      <c r="J130" t="s">
         <v>82</v>
       </c>
-      <c r="J130" t="s">
-        <v>83</v>
-      </c>
       <c r="K130" t="s">
         <v>19</v>
       </c>
@@ -5358,15 +5313,15 @@
         <v>74</v>
       </c>
     </row>
-    <row r="131" spans="1:14">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>13</v>
       </c>
-      <c r="B131" t="s">
-        <v>114</v>
-      </c>
-      <c r="C131" t="s">
-        <v>114</v>
+      <c r="B131">
+        <v>1022927</v>
+      </c>
+      <c r="C131">
+        <v>1022927</v>
       </c>
       <c r="D131" t="s">
         <v>14</v>
@@ -5375,14 +5330,14 @@
         <v>15</v>
       </c>
       <c r="F131" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="H131" t="s">
+        <v>81</v>
+      </c>
+      <c r="J131" t="s">
         <v>82</v>
       </c>
-      <c r="J131" t="s">
-        <v>83</v>
-      </c>
       <c r="K131" t="s">
         <v>19</v>
       </c>
@@ -5393,7 +5348,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="132" spans="1:14">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>39</v>
       </c>
@@ -5407,7 +5362,7 @@
         <v>15</v>
       </c>
       <c r="F132" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="H132" t="s">
         <v>72</v>
@@ -5425,7 +5380,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="133" spans="1:14">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>13</v>
       </c>
@@ -5445,11 +5400,11 @@
         <v>25</v>
       </c>
       <c r="H133" t="s">
+        <v>84</v>
+      </c>
+      <c r="J133" t="s">
         <v>85</v>
       </c>
-      <c r="J133" t="s">
-        <v>86</v>
-      </c>
       <c r="K133" t="s">
         <v>19</v>
       </c>
@@ -5460,15 +5415,15 @@
         <v>74</v>
       </c>
     </row>
-    <row r="134" spans="1:14">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>13</v>
       </c>
-      <c r="B134" t="s">
-        <v>117</v>
-      </c>
-      <c r="C134" t="s">
-        <v>117</v>
+      <c r="B134">
+        <v>1022928</v>
+      </c>
+      <c r="C134">
+        <v>1022928</v>
       </c>
       <c r="D134" t="s">
         <v>14</v>
@@ -5480,11 +5435,11 @@
         <v>25</v>
       </c>
       <c r="H134" t="s">
+        <v>81</v>
+      </c>
+      <c r="J134" t="s">
         <v>82</v>
       </c>
-      <c r="J134" t="s">
-        <v>83</v>
-      </c>
       <c r="K134" t="s">
         <v>19</v>
       </c>
@@ -5495,7 +5450,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="135" spans="1:14">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>13</v>
       </c>
@@ -5512,7 +5467,7 @@
         <v>15</v>
       </c>
       <c r="F135" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="H135" t="s">
         <v>72</v>
@@ -5530,7 +5485,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="136" spans="1:14">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>13</v>
       </c>
@@ -5550,11 +5505,11 @@
         <v>25</v>
       </c>
       <c r="H136" t="s">
+        <v>84</v>
+      </c>
+      <c r="J136" t="s">
         <v>85</v>
       </c>
-      <c r="J136" t="s">
-        <v>86</v>
-      </c>
       <c r="K136" t="s">
         <v>19</v>
       </c>
@@ -5565,15 +5520,15 @@
         <v>74</v>
       </c>
     </row>
-    <row r="137" spans="1:14">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>13</v>
       </c>
-      <c r="B137" t="s">
-        <v>119</v>
-      </c>
-      <c r="C137" t="s">
-        <v>119</v>
+      <c r="B137">
+        <v>1022932</v>
+      </c>
+      <c r="C137">
+        <v>1022932</v>
       </c>
       <c r="D137" t="s">
         <v>14</v>
@@ -5582,14 +5537,14 @@
         <v>15</v>
       </c>
       <c r="F137" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="H137" t="s">
+        <v>81</v>
+      </c>
+      <c r="J137" t="s">
         <v>82</v>
       </c>
-      <c r="J137" t="s">
-        <v>83</v>
-      </c>
       <c r="K137" t="s">
         <v>19</v>
       </c>
@@ -5600,7 +5555,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="138" spans="1:14">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>33</v>
       </c>
@@ -5614,13 +5569,13 @@
         <v>15</v>
       </c>
       <c r="F138" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="H138" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J138" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K138" t="s">
         <v>19</v>
@@ -5632,7 +5587,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="139" spans="1:14">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>13</v>
       </c>
@@ -5667,7 +5622,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="140" spans="1:14">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>13</v>
       </c>
@@ -5687,11 +5642,11 @@
         <v>44</v>
       </c>
       <c r="H140" t="s">
+        <v>84</v>
+      </c>
+      <c r="J140" t="s">
         <v>85</v>
       </c>
-      <c r="J140" t="s">
-        <v>86</v>
-      </c>
       <c r="K140" t="s">
         <v>19</v>
       </c>
@@ -5702,7 +5657,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="141" spans="1:14">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>13</v>
       </c>
@@ -5737,7 +5692,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="142" spans="1:14">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>13</v>
       </c>
@@ -5772,7 +5727,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="143" spans="1:14">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>13</v>
       </c>
@@ -5807,7 +5762,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="144" spans="1:14">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>30</v>
       </c>
@@ -5839,7 +5794,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="145" spans="1:14">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>13</v>
       </c>
@@ -5859,11 +5814,11 @@
         <v>29</v>
       </c>
       <c r="H145" t="s">
+        <v>84</v>
+      </c>
+      <c r="J145" t="s">
         <v>85</v>
       </c>
-      <c r="J145" t="s">
-        <v>86</v>
-      </c>
       <c r="K145" t="s">
         <v>19</v>
       </c>
@@ -5874,7 +5829,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="146" spans="1:14">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>13</v>
       </c>
@@ -5909,7 +5864,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="147" spans="1:14">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>39</v>
       </c>
@@ -5923,13 +5878,13 @@
         <v>15</v>
       </c>
       <c r="F147" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="H147" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J147" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K147" t="s">
         <v>19</v>
@@ -5941,7 +5896,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="148" spans="1:14">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>13</v>
       </c>
@@ -5961,10 +5916,10 @@
         <v>25</v>
       </c>
       <c r="H148" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J148" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K148" t="s">
         <v>19</v>
@@ -5976,7 +5931,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="149" spans="1:14">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>13</v>
       </c>
@@ -6011,7 +5966,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="150" spans="1:14">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>33</v>
       </c>
@@ -6025,7 +5980,7 @@
         <v>15</v>
       </c>
       <c r="F150" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="H150" t="s">
         <v>76</v>
@@ -6043,7 +5998,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="151" spans="1:14">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>33</v>
       </c>
@@ -6057,7 +6012,7 @@
         <v>15</v>
       </c>
       <c r="F151" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="H151" t="s">
         <v>72</v>
@@ -6075,7 +6030,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="152" spans="1:14">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>39</v>
       </c>
@@ -6089,7 +6044,7 @@
         <v>15</v>
       </c>
       <c r="F152" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="H152" t="s">
         <v>76</v>
@@ -6107,7 +6062,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="153" spans="1:14">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>13</v>
       </c>
@@ -6142,7 +6097,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="154" spans="1:14">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>13</v>
       </c>
@@ -6162,10 +6117,10 @@
         <v>44</v>
       </c>
       <c r="H154" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J154" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K154" t="s">
         <v>19</v>
@@ -6177,7 +6132,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="155" spans="1:14">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>13</v>
       </c>
@@ -6212,7 +6167,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="156" spans="1:14">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>30</v>
       </c>
@@ -6229,11 +6184,11 @@
         <v>25</v>
       </c>
       <c r="H156" t="s">
+        <v>81</v>
+      </c>
+      <c r="J156" t="s">
         <v>82</v>
       </c>
-      <c r="J156" t="s">
-        <v>83</v>
-      </c>
       <c r="K156" t="s">
         <v>19</v>
       </c>
@@ -6244,7 +6199,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="157" spans="1:14">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>13</v>
       </c>
@@ -6279,7 +6234,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="158" spans="1:14">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>13</v>
       </c>
@@ -6299,11 +6254,11 @@
         <v>25</v>
       </c>
       <c r="H158" t="s">
+        <v>84</v>
+      </c>
+      <c r="J158" t="s">
         <v>85</v>
       </c>
-      <c r="J158" t="s">
-        <v>86</v>
-      </c>
       <c r="K158" t="s">
         <v>19</v>
       </c>
@@ -6314,7 +6269,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="159" spans="1:14">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>13</v>
       </c>
@@ -6334,11 +6289,11 @@
         <v>25</v>
       </c>
       <c r="H159" t="s">
+        <v>84</v>
+      </c>
+      <c r="J159" t="s">
         <v>85</v>
       </c>
-      <c r="J159" t="s">
-        <v>86</v>
-      </c>
       <c r="K159" t="s">
         <v>19</v>
       </c>
@@ -6349,15 +6304,15 @@
         <v>74</v>
       </c>
     </row>
-    <row r="160" spans="1:14">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>13</v>
       </c>
-      <c r="B160" t="s">
-        <v>126</v>
-      </c>
-      <c r="C160" t="s">
-        <v>126</v>
+      <c r="B160">
+        <v>1022949</v>
+      </c>
+      <c r="C160">
+        <v>1022949</v>
       </c>
       <c r="D160" t="s">
         <v>14</v>
@@ -6366,14 +6321,14 @@
         <v>15</v>
       </c>
       <c r="F160" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="H160" t="s">
+        <v>81</v>
+      </c>
+      <c r="J160" t="s">
         <v>82</v>
       </c>
-      <c r="J160" t="s">
-        <v>83</v>
-      </c>
       <c r="K160" t="s">
         <v>19</v>
       </c>
@@ -6384,7 +6339,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="161" spans="1:14">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>39</v>
       </c>
@@ -6398,7 +6353,7 @@
         <v>15</v>
       </c>
       <c r="F161" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="H161" t="s">
         <v>79</v>
@@ -6416,7 +6371,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="162" spans="1:14">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>13</v>
       </c>
@@ -6451,7 +6406,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="163" spans="1:14">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>13</v>
       </c>
@@ -6471,10 +6426,10 @@
         <v>25</v>
       </c>
       <c r="H163" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J163" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K163" t="s">
         <v>19</v>
@@ -6486,7 +6441,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="164" spans="1:14">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>13</v>
       </c>
@@ -6506,10 +6461,10 @@
         <v>25</v>
       </c>
       <c r="H164" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J164" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K164" t="s">
         <v>19</v>
@@ -6521,15 +6476,15 @@
         <v>74</v>
       </c>
     </row>
-    <row r="165" spans="1:14">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>13</v>
       </c>
-      <c r="B165" t="s">
-        <v>129</v>
-      </c>
-      <c r="C165" t="s">
-        <v>129</v>
+      <c r="B165">
+        <v>1022934</v>
+      </c>
+      <c r="C165">
+        <v>1022934</v>
       </c>
       <c r="D165" t="s">
         <v>14</v>
@@ -6538,14 +6493,14 @@
         <v>15</v>
       </c>
       <c r="F165" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="H165" t="s">
+        <v>81</v>
+      </c>
+      <c r="J165" t="s">
         <v>82</v>
       </c>
-      <c r="J165" t="s">
-        <v>83</v>
-      </c>
       <c r="K165" t="s">
         <v>19</v>
       </c>
@@ -6556,15 +6511,15 @@
         <v>74</v>
       </c>
     </row>
-    <row r="166" spans="1:14">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>13</v>
       </c>
-      <c r="B166" t="s">
-        <v>131</v>
-      </c>
-      <c r="C166" t="s">
-        <v>131</v>
+      <c r="B166">
+        <v>1022946</v>
+      </c>
+      <c r="C166">
+        <v>1022946</v>
       </c>
       <c r="D166" t="s">
         <v>14</v>
@@ -6576,11 +6531,11 @@
         <v>25</v>
       </c>
       <c r="H166" t="s">
+        <v>81</v>
+      </c>
+      <c r="J166" t="s">
         <v>82</v>
       </c>
-      <c r="J166" t="s">
-        <v>83</v>
-      </c>
       <c r="K166" t="s">
         <v>19</v>
       </c>
@@ -6591,7 +6546,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="167" spans="1:14">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>13</v>
       </c>
@@ -6611,10 +6566,10 @@
         <v>25</v>
       </c>
       <c r="H167" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J167" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K167" t="s">
         <v>19</v>
@@ -6626,7 +6581,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="168" spans="1:14">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>13</v>
       </c>
@@ -6643,7 +6598,7 @@
         <v>15</v>
       </c>
       <c r="F168" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="H168" t="s">
         <v>79</v>
@@ -6661,7 +6616,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="169" spans="1:14">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>13</v>
       </c>
@@ -6696,7 +6651,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="170" spans="1:14">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>13</v>
       </c>
@@ -6731,7 +6686,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="171" spans="1:14">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>13</v>
       </c>
@@ -6748,7 +6703,7 @@
         <v>15</v>
       </c>
       <c r="F171" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="H171" t="s">
         <v>76</v>
@@ -6766,7 +6721,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="172" spans="1:14">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>13</v>
       </c>
@@ -6786,11 +6741,11 @@
         <v>25</v>
       </c>
       <c r="H172" t="s">
+        <v>84</v>
+      </c>
+      <c r="J172" t="s">
         <v>85</v>
       </c>
-      <c r="J172" t="s">
-        <v>86</v>
-      </c>
       <c r="K172" t="s">
         <v>19</v>
       </c>
@@ -6801,7 +6756,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="173" spans="1:14">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>13</v>
       </c>
@@ -6836,15 +6791,15 @@
         <v>74</v>
       </c>
     </row>
-    <row r="174" spans="1:14">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>13</v>
       </c>
-      <c r="B174" t="s">
-        <v>134</v>
-      </c>
-      <c r="C174" t="s">
-        <v>134</v>
+      <c r="B174">
+        <v>1022929</v>
+      </c>
+      <c r="C174">
+        <v>1022929</v>
       </c>
       <c r="D174" t="s">
         <v>14</v>
@@ -6853,14 +6808,14 @@
         <v>15</v>
       </c>
       <c r="F174" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="H174" t="s">
+        <v>81</v>
+      </c>
+      <c r="J174" t="s">
         <v>82</v>
       </c>
-      <c r="J174" t="s">
-        <v>83</v>
-      </c>
       <c r="K174" t="s">
         <v>19</v>
       </c>
@@ -6871,7 +6826,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="175" spans="1:14">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>39</v>
       </c>
@@ -6885,14 +6840,14 @@
         <v>15</v>
       </c>
       <c r="F175" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="H175" t="s">
+        <v>81</v>
+      </c>
+      <c r="J175" t="s">
         <v>82</v>
       </c>
-      <c r="J175" t="s">
-        <v>83</v>
-      </c>
       <c r="K175" t="s">
         <v>19</v>
       </c>
@@ -6903,15 +6858,15 @@
         <v>74</v>
       </c>
     </row>
-    <row r="176" spans="1:14">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>13</v>
       </c>
-      <c r="B176" t="s">
-        <v>137</v>
-      </c>
-      <c r="C176" t="s">
-        <v>137</v>
+      <c r="B176">
+        <v>1022937</v>
+      </c>
+      <c r="C176">
+        <v>1022937</v>
       </c>
       <c r="D176" t="s">
         <v>14</v>
@@ -6923,11 +6878,11 @@
         <v>25</v>
       </c>
       <c r="H176" t="s">
+        <v>81</v>
+      </c>
+      <c r="J176" t="s">
         <v>82</v>
       </c>
-      <c r="J176" t="s">
-        <v>83</v>
-      </c>
       <c r="K176" t="s">
         <v>19</v>
       </c>
@@ -6938,7 +6893,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="177" spans="1:14">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>13</v>
       </c>
@@ -6973,7 +6928,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="178" spans="1:14">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>13</v>
       </c>
@@ -7008,7 +6963,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="179" spans="1:14">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>33</v>
       </c>
@@ -7022,14 +6977,14 @@
         <v>15</v>
       </c>
       <c r="F179" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="H179" t="s">
+        <v>81</v>
+      </c>
+      <c r="J179" t="s">
         <v>82</v>
       </c>
-      <c r="J179" t="s">
-        <v>83</v>
-      </c>
       <c r="K179" t="s">
         <v>19</v>
       </c>
@@ -7040,7 +6995,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="180" spans="1:14">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>30</v>
       </c>
@@ -7072,7 +7027,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="181" spans="1:14">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>30</v>
       </c>
@@ -7104,7 +7059,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="182" spans="1:14">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>13</v>
       </c>
@@ -7121,7 +7076,7 @@
         <v>15</v>
       </c>
       <c r="F182" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="H182" t="s">
         <v>76</v>
@@ -7139,7 +7094,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="183" spans="1:14">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>13</v>
       </c>
@@ -7174,7 +7129,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="184" spans="1:14">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>13</v>
       </c>
@@ -7191,7 +7146,7 @@
         <v>15</v>
       </c>
       <c r="F184" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="H184" t="s">
         <v>79</v>
@@ -7209,7 +7164,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="185" spans="1:14">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>13</v>
       </c>
@@ -7229,11 +7184,11 @@
         <v>25</v>
       </c>
       <c r="H185" t="s">
+        <v>84</v>
+      </c>
+      <c r="J185" t="s">
         <v>85</v>
       </c>
-      <c r="J185" t="s">
-        <v>86</v>
-      </c>
       <c r="K185" t="s">
         <v>19</v>
       </c>
@@ -7244,7 +7199,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="186" spans="1:14">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>39</v>
       </c>
@@ -7258,14 +7213,14 @@
         <v>15</v>
       </c>
       <c r="F186" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="H186" t="s">
+        <v>84</v>
+      </c>
+      <c r="J186" t="s">
         <v>85</v>
       </c>
-      <c r="J186" t="s">
-        <v>86</v>
-      </c>
       <c r="K186" t="s">
         <v>19</v>
       </c>
@@ -7276,7 +7231,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="187" spans="1:14">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>13</v>
       </c>
@@ -7296,10 +7251,10 @@
         <v>29</v>
       </c>
       <c r="H187" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J187" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K187" t="s">
         <v>19</v>
@@ -7311,7 +7266,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="188" spans="1:14">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>13</v>
       </c>
@@ -7328,7 +7283,7 @@
         <v>15</v>
       </c>
       <c r="F188" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="H188" t="s">
         <v>79</v>
@@ -7346,7 +7301,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="189" spans="1:14">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>13</v>
       </c>
@@ -7366,10 +7321,10 @@
         <v>25</v>
       </c>
       <c r="H189" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J189" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K189" t="s">
         <v>19</v>
@@ -7381,7 +7336,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="190" spans="1:14">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>30</v>
       </c>
@@ -7398,11 +7353,11 @@
         <v>25</v>
       </c>
       <c r="H190" t="s">
+        <v>84</v>
+      </c>
+      <c r="J190" t="s">
         <v>85</v>
       </c>
-      <c r="J190" t="s">
-        <v>86</v>
-      </c>
       <c r="K190" t="s">
         <v>19</v>
       </c>
@@ -7413,7 +7368,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="191" spans="1:14">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>13</v>
       </c>
@@ -7448,7 +7403,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="192" spans="1:14">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>13</v>
       </c>
@@ -7483,7 +7438,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="193" spans="1:14">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>13</v>
       </c>
@@ -7518,7 +7473,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="194" spans="1:14">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>13</v>
       </c>
@@ -7553,7 +7508,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="195" spans="1:14">
+    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>13</v>
       </c>
@@ -7588,15 +7543,15 @@
         <v>74</v>
       </c>
     </row>
-    <row r="196" spans="1:14">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>13</v>
       </c>
-      <c r="B196" t="s">
-        <v>143</v>
-      </c>
-      <c r="C196" t="s">
-        <v>143</v>
+      <c r="B196">
+        <v>1022943</v>
+      </c>
+      <c r="C196">
+        <v>1022943</v>
       </c>
       <c r="D196" t="s">
         <v>14</v>
@@ -7608,11 +7563,11 @@
         <v>25</v>
       </c>
       <c r="H196" t="s">
+        <v>81</v>
+      </c>
+      <c r="J196" t="s">
         <v>82</v>
       </c>
-      <c r="J196" t="s">
-        <v>83</v>
-      </c>
       <c r="K196" t="s">
         <v>19</v>
       </c>
@@ -7623,7 +7578,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="197" spans="1:14">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>13</v>
       </c>
@@ -7640,13 +7595,13 @@
         <v>15</v>
       </c>
       <c r="F197" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="H197" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J197" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K197" t="s">
         <v>19</v>
@@ -7658,7 +7613,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="198" spans="1:14">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>13</v>
       </c>
@@ -7675,14 +7630,14 @@
         <v>15</v>
       </c>
       <c r="F198" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="H198" t="s">
+        <v>84</v>
+      </c>
+      <c r="J198" t="s">
         <v>85</v>
       </c>
-      <c r="J198" t="s">
-        <v>86</v>
-      </c>
       <c r="K198" t="s">
         <v>19</v>
       </c>
@@ -7693,7 +7648,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="199" spans="1:14">
+    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>13</v>
       </c>
@@ -7728,7 +7683,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="200" spans="1:14">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>13</v>
       </c>
@@ -7763,7 +7718,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="201" spans="1:14">
+    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>13</v>
       </c>
@@ -7798,7 +7753,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="202" spans="1:14">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>13</v>
       </c>
@@ -7833,7 +7788,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="203" spans="1:14">
+    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>13</v>
       </c>
@@ -7853,10 +7808,10 @@
         <v>29</v>
       </c>
       <c r="H203" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J203" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K203" t="s">
         <v>19</v>
@@ -7868,7 +7823,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="204" spans="1:14">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>13</v>
       </c>
@@ -7885,13 +7840,13 @@
         <v>15</v>
       </c>
       <c r="F204" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="H204" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J204" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K204" t="s">
         <v>19</v>
@@ -7903,15 +7858,15 @@
         <v>74</v>
       </c>
     </row>
-    <row r="205" spans="1:14">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>13</v>
       </c>
-      <c r="B205" t="s">
-        <v>147</v>
-      </c>
-      <c r="C205" t="s">
-        <v>147</v>
+      <c r="B205">
+        <v>1022945</v>
+      </c>
+      <c r="C205">
+        <v>1022945</v>
       </c>
       <c r="D205" t="s">
         <v>14</v>
@@ -7920,14 +7875,14 @@
         <v>15</v>
       </c>
       <c r="F205" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="H205" t="s">
+        <v>81</v>
+      </c>
+      <c r="J205" t="s">
         <v>82</v>
       </c>
-      <c r="J205" t="s">
-        <v>83</v>
-      </c>
       <c r="K205" t="s">
         <v>19</v>
       </c>
@@ -7938,7 +7893,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="206" spans="1:14">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>13</v>
       </c>
@@ -7955,7 +7910,7 @@
         <v>15</v>
       </c>
       <c r="F206" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="H206" t="s">
         <v>76</v>
@@ -7973,7 +7928,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="207" spans="1:14">
+    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>13</v>
       </c>
@@ -8008,7 +7963,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="208" spans="1:14">
+    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>13</v>
       </c>
@@ -8028,10 +7983,10 @@
         <v>25</v>
       </c>
       <c r="H208" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J208" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K208" t="s">
         <v>19</v>
@@ -8043,7 +7998,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="209" spans="1:14">
+    <row r="209" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>13</v>
       </c>
@@ -8078,15 +8033,15 @@
         <v>74</v>
       </c>
     </row>
-    <row r="210" spans="1:14">
+    <row r="210" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>13</v>
       </c>
-      <c r="B210" t="s">
-        <v>149</v>
-      </c>
-      <c r="C210" t="s">
-        <v>149</v>
+      <c r="B210">
+        <v>1022948</v>
+      </c>
+      <c r="C210">
+        <v>1022948</v>
       </c>
       <c r="D210" t="s">
         <v>14</v>
@@ -8095,14 +8050,14 @@
         <v>15</v>
       </c>
       <c r="F210" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="H210" t="s">
+        <v>81</v>
+      </c>
+      <c r="J210" t="s">
         <v>82</v>
       </c>
-      <c r="J210" t="s">
-        <v>83</v>
-      </c>
       <c r="K210" t="s">
         <v>19</v>
       </c>
@@ -8113,7 +8068,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="211" spans="1:14">
+    <row r="211" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>13</v>
       </c>
@@ -8130,13 +8085,13 @@
         <v>15</v>
       </c>
       <c r="F211" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="H211" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J211" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K211" t="s">
         <v>19</v>
@@ -8148,7 +8103,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="212" spans="1:14">
+    <row r="212" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>13</v>
       </c>
@@ -8165,14 +8120,14 @@
         <v>15</v>
       </c>
       <c r="F212" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="H212" t="s">
+        <v>84</v>
+      </c>
+      <c r="J212" t="s">
         <v>85</v>
       </c>
-      <c r="J212" t="s">
-        <v>86</v>
-      </c>
       <c r="K212" t="s">
         <v>19</v>
       </c>
@@ -8183,7 +8138,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="213" spans="1:14">
+    <row r="213" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>13</v>
       </c>
@@ -8200,7 +8155,7 @@
         <v>15</v>
       </c>
       <c r="F213" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="H213" t="s">
         <v>79</v>
@@ -8218,7 +8173,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="214" spans="1:14">
+    <row r="214" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>13</v>
       </c>
@@ -8238,11 +8193,11 @@
         <v>25</v>
       </c>
       <c r="H214" t="s">
+        <v>84</v>
+      </c>
+      <c r="J214" t="s">
         <v>85</v>
       </c>
-      <c r="J214" t="s">
-        <v>86</v>
-      </c>
       <c r="K214" t="s">
         <v>19</v>
       </c>
@@ -8253,7 +8208,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="215" spans="1:14">
+    <row r="215" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>13</v>
       </c>
@@ -8270,14 +8225,14 @@
         <v>15</v>
       </c>
       <c r="F215" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="H215" t="s">
+        <v>84</v>
+      </c>
+      <c r="J215" t="s">
         <v>85</v>
       </c>
-      <c r="J215" t="s">
-        <v>86</v>
-      </c>
       <c r="K215" t="s">
         <v>19</v>
       </c>
@@ -8288,31 +8243,21 @@
         <v>74</v>
       </c>
     </row>
-    <row r="216" spans="1:14">
+    <row r="216" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="N216" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="217" spans="1:14">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="217" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M217" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>